<commit_message>
feat : end of transmitter script
- end of transmitter python script
</commit_message>
<xml_diff>
--- a/software/clées.xlsx
+++ b/software/clées.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sylvain\Desktop\Projets\PC_controller\software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88A2FE9-EE52-40D8-BC53-9C120708AF84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CC66A0-5444-4E3A-AA22-0601CE789387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="0" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>WEB API KEY</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>a35df02ffc4b9fadd1b3ec977fc3b3</t>
+  </si>
+  <si>
+    <t>actions</t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power </t>
+  </si>
+  <si>
+    <t>0x02</t>
+  </si>
+  <si>
+    <t>reset</t>
   </si>
 </sst>
 </file>
@@ -354,19 +369,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="60.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,12 +390,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AVR : support of 2 way HC12
</commit_message>
<xml_diff>
--- a/software/clées.xlsx
+++ b/software/clées.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sylvain\Desktop\Projets\PC_controller\software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CC66A0-5444-4E3A-AA22-0601CE789387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489F1C39-8D63-4D7F-9410-DAE07127FD96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>WEB API KEY</t>
   </si>
@@ -52,6 +52,36 @@
   </si>
   <si>
     <t>reset</t>
+  </si>
+  <si>
+    <t>0x03</t>
+  </si>
+  <si>
+    <t>battery level callback</t>
+  </si>
+  <si>
+    <t>avr--&gt;server</t>
+  </si>
+  <si>
+    <t>ready for transmission</t>
+  </si>
+  <si>
+    <t>bad action</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>bad key</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>battery level transmission (2 bytes)</t>
   </si>
 </sst>
 </file>
@@ -369,17 +399,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -417,6 +447,57 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
AVR : realease code
debug complete
</commit_message>
<xml_diff>
--- a/software/clées.xlsx
+++ b/software/clées.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sylvain\Desktop\Projets\PC_controller\software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489F1C39-8D63-4D7F-9410-DAE07127FD96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D52895-339F-4E84-85A7-9DCFE0367F4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>WEB API KEY</t>
   </si>
@@ -36,52 +36,52 @@
     <t>a067db7c-bffd-4f26-8151-20a487679dc3</t>
   </si>
   <si>
-    <t>a35df02ffc4b9fadd1b3ec977fc3b3</t>
-  </si>
-  <si>
     <t>actions</t>
   </si>
   <si>
-    <t>0x01</t>
-  </si>
-  <si>
     <t xml:space="preserve">power </t>
   </si>
   <si>
-    <t>0x02</t>
-  </si>
-  <si>
     <t>reset</t>
   </si>
   <si>
-    <t>0x03</t>
-  </si>
-  <si>
     <t>battery level callback</t>
   </si>
   <si>
     <t>avr--&gt;server</t>
   </si>
   <si>
-    <t>ready for transmission</t>
-  </si>
-  <si>
     <t>bad action</t>
   </si>
   <si>
-    <t>0x04</t>
-  </si>
-  <si>
     <t>bad key</t>
   </si>
   <si>
-    <t>0x05</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
     <t>battery level transmission (2 bytes)</t>
+  </si>
+  <si>
+    <t>b (0x62)</t>
+  </si>
+  <si>
+    <t>a (0x61)</t>
+  </si>
+  <si>
+    <t>k (0x6b)</t>
+  </si>
+  <si>
+    <t>o (0x6f)</t>
+  </si>
+  <si>
+    <t>p (0x70)</t>
+  </si>
+  <si>
+    <t>r (0x72)</t>
+  </si>
+  <si>
+    <t>a35df02ffc4b9fadd1b3</t>
   </si>
 </sst>
 </file>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,77 +425,69 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
         <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>